<commit_message>
Figure to PCA journal.
</commit_message>
<xml_diff>
--- a/Data/Firts_LCMS_Metabolite_HeatMap.xlsx
+++ b/Data/Firts_LCMS_Metabolite_HeatMap.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8954" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8954" uniqueCount="1967">
   <si>
     <t xml:space="preserve">Sample_ID</t>
   </si>
@@ -5913,6 +5913,9 @@
   </si>
   <si>
     <t xml:space="preserve">7795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glucose</t>
   </si>
   <si>
     <t xml:space="preserve">Pyrocatechuic acid</t>
@@ -70037,7 +70040,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>129</v>
+        <v>1964</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>102</v>
@@ -70269,7 +70272,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>88</v>
@@ -70298,7 +70301,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>88</v>

</xml_diff>